<commit_message>
Update KSR 1 - added legend
</commit_message>
<xml_diff>
--- a/TestCases-KSR.xlsx
+++ b/TestCases-KSR.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Mirugin\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="23040" windowHeight="8700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="Сценарии тестирования" sheetId="1" r:id="rId1"/>
+    <sheet name="Легенда" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="Status">'[1]Тестовые данные'!#REF!</definedName>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="152">
   <si>
     <t>V1.0</t>
   </si>
@@ -510,12 +516,96 @@
   <si>
     <t>Ввод не уникального значения</t>
   </si>
+  <si>
+    <t>Автор</t>
+  </si>
+  <si>
+    <t>Создание документа</t>
+  </si>
+  <si>
+    <t>V1.0.0</t>
+  </si>
+  <si>
+    <t>дата</t>
+  </si>
+  <si>
+    <t>Описание изменений</t>
+  </si>
+  <si>
+    <t>Версия</t>
+  </si>
+  <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>История изменений</t>
+  </si>
+  <si>
+    <t>Недоступно для тестирования / функция не имплементирована</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Тест ОК, функция работает стабильно</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OK</t>
+  </si>
+  <si>
+    <t>Обнаружены дефекты со статусами: Важный, Средний, Незначительный</t>
+  </si>
+  <si>
+    <t>&lt;Issue ID&gt;</t>
+  </si>
+  <si>
+    <t>Обнаружены критические дефекты</t>
+  </si>
+  <si>
+    <t>Вопросы по функциональности, тест отложен</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Обозначение результатов тестирования</t>
+  </si>
+  <si>
+    <t>"Спецификация_документ.doc" - спецификация требований.</t>
+  </si>
+  <si>
+    <t>Ссылки:</t>
+  </si>
+  <si>
+    <t>&lt;компания&gt;</t>
+  </si>
+  <si>
+    <t>Предоставил:</t>
+  </si>
+  <si>
+    <t>Предоставлено для:</t>
+  </si>
+  <si>
+    <t>Проектная команда тестирования, менеджеры проекта, Заказчик</t>
+  </si>
+  <si>
+    <t>Аудитория:</t>
+  </si>
+  <si>
+    <t>Список проверок для функционального/регрессионного тестирования</t>
+  </si>
+  <si>
+    <t>Система &lt;название&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  </numFmts>
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,8 +681,58 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -635,8 +775,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -822,12 +991,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -894,6 +1084,9 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -927,13 +1120,100 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1020,7 +1300,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1055,7 +1335,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1273,21 +1553,21 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>119</v>
       </c>
@@ -1307,7 +1587,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1315,21 +1595,21 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="33"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="34"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>39</v>
       </c>
@@ -1389,19 +1669,19 @@
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="36"/>
-    </row>
-    <row r="5" spans="1:16" ht="165.75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="37"/>
+    </row>
+    <row r="5" spans="1:16" ht="171.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1429,7 +1709,7 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
@@ -1457,7 +1737,7 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:16" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>40</v>
       </c>
@@ -1487,7 +1767,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:16" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>41</v>
       </c>
@@ -1517,7 +1797,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
-    <row r="9" spans="1:16" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="26.4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>43</v>
       </c>
@@ -1547,7 +1827,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>42</v>
       </c>
@@ -1557,19 +1837,19 @@
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="36"/>
-    </row>
-    <row r="11" spans="1:16" ht="153" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="37"/>
+    </row>
+    <row r="11" spans="1:16" ht="158.4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>44</v>
       </c>
@@ -1597,11 +1877,11 @@
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
     </row>
-    <row r="12" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="20" t="s">
@@ -1627,9 +1907,9 @@
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
     </row>
-    <row r="13" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="30"/>
+    <row r="13" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="20" t="s">
         <v>50</v>
       </c>
@@ -1639,7 +1919,7 @@
       <c r="E13" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="26" t="s">
         <v>123</v>
       </c>
       <c r="G13" s="22"/>
@@ -1653,9 +1933,9 @@
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
     </row>
-    <row r="14" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="30"/>
+    <row r="14" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="20" t="s">
         <v>51</v>
       </c>
@@ -1679,9 +1959,9 @@
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
     </row>
-    <row r="15" spans="1:16" s="23" customFormat="1" ht="102" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="30"/>
+    <row r="15" spans="1:16" s="23" customFormat="1" ht="105.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="20" t="s">
         <v>52</v>
       </c>
@@ -1705,9 +1985,9 @@
       <c r="O15" s="22"/>
       <c r="P15" s="22"/>
     </row>
-    <row r="16" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="30"/>
+    <row r="16" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="20" t="s">
         <v>53</v>
       </c>
@@ -1731,9 +2011,9 @@
       <c r="O16" s="22"/>
       <c r="P16" s="22"/>
     </row>
-    <row r="17" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="30"/>
+    <row r="17" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="20" t="s">
         <v>54</v>
       </c>
@@ -1757,9 +2037,9 @@
       <c r="O17" s="22"/>
       <c r="P17" s="22"/>
     </row>
-    <row r="18" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="30"/>
+    <row r="18" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="20" t="s">
         <v>55</v>
       </c>
@@ -1783,9 +2063,9 @@
       <c r="O18" s="22"/>
       <c r="P18" s="22"/>
     </row>
-    <row r="19" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="30"/>
+    <row r="19" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="20" t="s">
         <v>69</v>
       </c>
@@ -1808,9 +2088,9 @@
       <c r="O19" s="22"/>
       <c r="P19" s="22"/>
     </row>
-    <row r="20" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="30"/>
+    <row r="20" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="20" t="s">
         <v>70</v>
       </c>
@@ -1834,9 +2114,9 @@
       <c r="O20" s="22"/>
       <c r="P20" s="22"/>
     </row>
-    <row r="21" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="30"/>
+    <row r="21" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="20" t="s">
         <v>58</v>
       </c>
@@ -1860,9 +2140,9 @@
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
     </row>
-    <row r="22" spans="1:16" s="23" customFormat="1" ht="76.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="30"/>
+    <row r="22" spans="1:16" s="23" customFormat="1" ht="79.2" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="20" t="s">
         <v>59</v>
       </c>
@@ -1886,9 +2166,9 @@
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
     </row>
-    <row r="23" spans="1:16" s="23" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="30"/>
+    <row r="23" spans="1:16" s="23" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="20" t="s">
         <v>60</v>
       </c>
@@ -1912,9 +2192,9 @@
       <c r="O23" s="22"/>
       <c r="P23" s="22"/>
     </row>
-    <row r="24" spans="1:16" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="31"/>
+    <row r="24" spans="1:16" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="20" t="s">
         <v>124</v>
       </c>
@@ -1938,11 +2218,11 @@
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
     </row>
-    <row r="25" spans="1:16" s="23" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:16" s="23" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="30" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="20" t="s">
@@ -1968,9 +2248,9 @@
       <c r="O25" s="22"/>
       <c r="P25" s="22"/>
     </row>
-    <row r="26" spans="1:16" s="23" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="30"/>
+    <row r="26" spans="1:16" s="23" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="20" t="s">
         <v>50</v>
       </c>
@@ -1994,9 +2274,9 @@
       <c r="O26" s="22"/>
       <c r="P26" s="22"/>
     </row>
-    <row r="27" spans="1:16" s="23" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="30"/>
+    <row r="27" spans="1:16" s="23" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="28"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="20" t="s">
         <v>51</v>
       </c>
@@ -2020,9 +2300,9 @@
       <c r="O27" s="22"/>
       <c r="P27" s="22"/>
     </row>
-    <row r="28" spans="1:16" s="23" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="30"/>
+    <row r="28" spans="1:16" s="23" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="20" t="s">
         <v>52</v>
       </c>
@@ -2046,9 +2326,9 @@
       <c r="O28" s="22"/>
       <c r="P28" s="22"/>
     </row>
-    <row r="29" spans="1:16" s="23" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="30"/>
+    <row r="29" spans="1:16" s="23" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="20" t="s">
         <v>53</v>
       </c>
@@ -2072,9 +2352,9 @@
       <c r="O29" s="22"/>
       <c r="P29" s="22"/>
     </row>
-    <row r="30" spans="1:16" s="23" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="30"/>
+    <row r="30" spans="1:16" s="23" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="20" t="s">
         <v>54</v>
       </c>
@@ -2098,9 +2378,9 @@
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
     </row>
-    <row r="31" spans="1:16" s="23" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="30"/>
+    <row r="31" spans="1:16" s="23" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="28"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="20" t="s">
         <v>55</v>
       </c>
@@ -2124,9 +2404,9 @@
       <c r="O31" s="22"/>
       <c r="P31" s="22"/>
     </row>
-    <row r="32" spans="1:16" s="23" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="30"/>
+    <row r="32" spans="1:16" s="23" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="20" t="s">
         <v>87</v>
       </c>
@@ -2149,9 +2429,9 @@
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
     </row>
-    <row r="33" spans="1:16" s="23" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="30"/>
+    <row r="33" spans="1:16" s="23" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="28"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="20" t="s">
         <v>88</v>
       </c>
@@ -2175,9 +2455,9 @@
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
     </row>
-    <row r="34" spans="1:16" s="23" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="30"/>
+    <row r="34" spans="1:16" s="23" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="28"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="20" t="s">
         <v>58</v>
       </c>
@@ -2201,9 +2481,9 @@
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
     </row>
-    <row r="35" spans="1:16" s="23" customFormat="1" ht="76.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="30"/>
+    <row r="35" spans="1:16" s="23" customFormat="1" ht="79.2" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="20" t="s">
         <v>59</v>
       </c>
@@ -2227,9 +2507,9 @@
       <c r="O35" s="22"/>
       <c r="P35" s="22"/>
     </row>
-    <row r="36" spans="1:16" s="23" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="30"/>
+    <row r="36" spans="1:16" s="23" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="28"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="20" t="s">
         <v>60</v>
       </c>
@@ -2253,9 +2533,9 @@
       <c r="O36" s="22"/>
       <c r="P36" s="22"/>
     </row>
-    <row r="37" spans="1:16" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="31"/>
+    <row r="37" spans="1:16" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="29"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="20" t="s">
         <v>124</v>
       </c>
@@ -2279,11 +2559,11 @@
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
     </row>
-    <row r="38" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+    <row r="38" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="30" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="20" t="s">
@@ -2309,9 +2589,9 @@
       <c r="O38" s="22"/>
       <c r="P38" s="22"/>
     </row>
-    <row r="39" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="30"/>
+    <row r="39" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="28"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="20" t="s">
         <v>50</v>
       </c>
@@ -2335,9 +2615,9 @@
       <c r="O39" s="22"/>
       <c r="P39" s="22"/>
     </row>
-    <row r="40" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="30"/>
+    <row r="40" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="20" t="s">
         <v>51</v>
       </c>
@@ -2361,9 +2641,9 @@
       <c r="O40" s="22"/>
       <c r="P40" s="22"/>
     </row>
-    <row r="41" spans="1:16" s="23" customFormat="1" ht="102" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="30"/>
+    <row r="41" spans="1:16" s="23" customFormat="1" ht="105.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="20" t="s">
         <v>52</v>
       </c>
@@ -2387,9 +2667,9 @@
       <c r="O41" s="22"/>
       <c r="P41" s="22"/>
     </row>
-    <row r="42" spans="1:16" s="23" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="30"/>
+    <row r="42" spans="1:16" s="23" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="20" t="s">
         <v>53</v>
       </c>
@@ -2413,9 +2693,9 @@
       <c r="O42" s="22"/>
       <c r="P42" s="22"/>
     </row>
-    <row r="43" spans="1:16" s="23" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="30"/>
+    <row r="43" spans="1:16" s="23" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="20" t="s">
         <v>54</v>
       </c>
@@ -2439,9 +2719,9 @@
       <c r="O43" s="22"/>
       <c r="P43" s="22"/>
     </row>
-    <row r="44" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
-      <c r="B44" s="30"/>
+    <row r="44" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="28"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="20" t="s">
         <v>55</v>
       </c>
@@ -2465,9 +2745,9 @@
       <c r="O44" s="22"/>
       <c r="P44" s="22"/>
     </row>
-    <row r="45" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="30"/>
+    <row r="45" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="20" t="s">
         <v>56</v>
       </c>
@@ -2490,9 +2770,9 @@
       <c r="O45" s="22"/>
       <c r="P45" s="22"/>
     </row>
-    <row r="46" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
-      <c r="B46" s="30"/>
+    <row r="46" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="28"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="20" t="s">
         <v>57</v>
       </c>
@@ -2516,9 +2796,9 @@
       <c r="O46" s="22"/>
       <c r="P46" s="22"/>
     </row>
-    <row r="47" spans="1:16" s="23" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
-      <c r="B47" s="30"/>
+    <row r="47" spans="1:16" s="23" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="28"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="20" t="s">
         <v>58</v>
       </c>
@@ -2542,9 +2822,9 @@
       <c r="O47" s="22"/>
       <c r="P47" s="22"/>
     </row>
-    <row r="48" spans="1:16" s="23" customFormat="1" ht="76.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
-      <c r="B48" s="30"/>
+    <row r="48" spans="1:16" s="23" customFormat="1" ht="79.2" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="28"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="20" t="s">
         <v>59</v>
       </c>
@@ -2568,9 +2848,9 @@
       <c r="O48" s="22"/>
       <c r="P48" s="22"/>
     </row>
-    <row r="49" spans="1:16" s="23" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
-      <c r="B49" s="30"/>
+    <row r="49" spans="1:16" s="23" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="28"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="20" t="s">
         <v>60</v>
       </c>
@@ -2594,7 +2874,7 @@
       <c r="O49" s="22"/>
       <c r="P49" s="22"/>
     </row>
-    <row r="50" spans="1:16" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>105</v>
       </c>
@@ -2622,7 +2902,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" spans="1:16" s="23" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="23" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
         <v>109</v>
       </c>
@@ -2650,7 +2930,7 @@
       <c r="O51" s="22"/>
       <c r="P51" s="22"/>
     </row>
-    <row r="52" spans="1:16" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="26.4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>110</v>
       </c>
@@ -2678,7 +2958,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="13"/>
     </row>
-    <row r="53" spans="1:16" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>114</v>
       </c>
@@ -2708,7 +2988,7 @@
       <c r="O53" s="13"/>
       <c r="P53" s="13"/>
     </row>
-    <row r="54" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
       <c r="B54" s="18"/>
       <c r="C54" s="12"/>
@@ -2726,7 +3006,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="13"/>
     </row>
-    <row r="55" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
       <c r="B55" s="18"/>
       <c r="C55" s="12"/>
@@ -2744,7 +3024,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="13"/>
     </row>
-    <row r="56" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
       <c r="B56" s="18"/>
       <c r="C56" s="20"/>
@@ -2762,7 +3042,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="13"/>
     </row>
-    <row r="57" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
       <c r="B57" s="18"/>
       <c r="C57" s="20"/>
@@ -2780,7 +3060,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="13"/>
     </row>
-    <row r="58" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
       <c r="B58" s="21"/>
       <c r="C58" s="20"/>
@@ -2821,4 +3101,200 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="55.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+    </row>
+    <row r="2" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+    </row>
+    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+    </row>
+    <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="64"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="65"/>
+      <c r="D6" s="64"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="60"/>
+    </row>
+    <row r="8" spans="1:7" s="57" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="58"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="50"/>
+      <c r="D9" s="49"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="D10" s="49"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="49"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="50"/>
+      <c r="D12" s="49"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="49"/>
+    </row>
+    <row r="14" spans="1:7" s="38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="46"/>
+    </row>
+    <row r="15" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>